<commit_message>
More report generation refinement
</commit_message>
<xml_diff>
--- a/reportTemplate.xlsx
+++ b/reportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (ABiL)\ABiL Team Folder\SharedFolder\Projects\CDC-Jonas-URDO\FilesForBiolinux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53DCE19-FC22-48BD-B643-FABBB66B8761}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85152946-5A50-48C9-92AE-CD0ABCB82CAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7500" xr2:uid="{8A14C74E-A60C-41DA-B532-3BADC25E42A8}"/>
   </bookViews>
@@ -54,21 +54,12 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Percent of total reads</t>
-  </si>
-  <si>
     <t>Type / Resistance</t>
   </si>
   <si>
     <t>Family</t>
   </si>
   <si>
-    <t xml:space="preserve">Genus </t>
-  </si>
-  <si>
-    <t>No Rank</t>
-  </si>
-  <si>
     <t>Drug resistance</t>
   </si>
   <si>
@@ -76,6 +67,15 @@
   </si>
   <si>
     <t>Virus</t>
+  </si>
+  <si>
+    <t>Species / Common Name</t>
+  </si>
+  <si>
+    <t># of reads</t>
+  </si>
+  <si>
+    <t>% of reads</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -158,30 +158,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -206,57 +186,59 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,238 +553,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67E829A-532F-4D99-B9FA-090A92809A14}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="16" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="D16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="E1:I1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
So pretty, so fine.
</commit_message>
<xml_diff>
--- a/reportTemplate.xlsx
+++ b/reportTemplate.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (ABiL)\ABiL Team Folder\SharedFolder\Projects\CDC-Jonas-URDO\FilesForBiolinux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\againes9\AppData\Local\Temp\scp58257\storage\projects\cdc-urdo\smored\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85152946-5A50-48C9-92AE-CD0ABCB82CAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7500" xr2:uid="{8A14C74E-A60C-41DA-B532-3BADC25E42A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Sample:</t>
   </si>
   <si>
-    <t>Total # of reads sequences</t>
-  </si>
-  <si>
     <t>Total # of merged reads:</t>
   </si>
   <si>
@@ -63,26 +59,29 @@
     <t>Drug resistance</t>
   </si>
   <si>
-    <t>Common name</t>
-  </si>
-  <si>
     <t>Virus</t>
   </si>
   <si>
-    <t>Species / Common Name</t>
-  </si>
-  <si>
     <t># of reads</t>
   </si>
   <si>
     <t>% of reads</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Total # of reads sequences:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +107,32 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -190,11 +215,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -202,43 +224,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,6 +287,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>957943</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7459980" y="0"/>
+          <a:ext cx="881743" cy="411480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,203 +634,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67E829A-532F-4D99-B9FA-090A92809A14}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:6" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="C14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="D14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="8"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>